<commit_message>
Updated gravity comp and electrical connection spreadsheet
</commit_message>
<xml_diff>
--- a/doc/Frc2019ElectricalConnectors.xlsx
+++ b/doc/Frc2019ElectricalConnectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Trc492\Frc2019DestinationDeepSpace\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhay\Documents\GitHub\Frc2019DestinationDeepSpace\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83C8466-C18D-4222-96F6-65368A295BAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33420288-7B69-46A3-B4F1-3175568FD4B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="615" windowWidth="21600" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors Checklist" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="111">
   <si>
     <t>Color</t>
   </si>
@@ -379,7 +379,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +440,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -453,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -499,6 +523,14 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,15 +925,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -909,78 +943,78 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="29" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="30" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>100</v>
       </c>
@@ -999,26 +1033,26 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1044,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -1065,7 +1099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1086,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1107,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
@@ -1129,7 +1163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1141,7 +1175,7 @@
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1153,7 +1187,7 @@
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1165,7 +1199,7 @@
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1177,10 +1211,10 @@
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1192,7 +1226,7 @@
       </c>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1204,7 +1238,7 @@
       </c>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1216,7 +1250,7 @@
       </c>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1229,7 +1263,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1241,7 +1275,7 @@
       </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -1253,7 +1287,7 @@
       </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1265,7 +1299,7 @@
       </c>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1277,10 +1311,10 @@
       </c>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -1292,7 +1326,7 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1304,7 +1338,7 @@
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1316,7 +1350,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1363,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -1341,7 +1375,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1353,7 +1387,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -1365,7 +1399,7 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -1380,10 +1414,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1398,7 +1432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -1419,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1440,7 +1474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -1462,7 +1496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1483,7 +1517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1501,7 +1535,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -1522,7 +1556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1534,13 +1568,13 @@
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="H37" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -1569,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -1595,7 +1629,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
@@ -1624,7 +1658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -1653,7 +1687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
@@ -1673,7 +1707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>68</v>
       </c>
@@ -1696,7 +1730,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
@@ -1725,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
@@ -1754,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="H46" s="2">
         <v>2</v>
@@ -1763,7 +1797,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>69</v>
       </c>
@@ -1783,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>69</v>
       </c>
@@ -1806,7 +1840,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>69</v>
       </c>
@@ -1835,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>69</v>
       </c>
@@ -1864,7 +1898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>69</v>
       </c>
@@ -1890,7 +1924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>69</v>
       </c>
@@ -1910,7 +1944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
@@ -1930,7 +1964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>69</v>
       </c>
@@ -1950,10 +1984,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>42</v>
       </c>
@@ -1973,7 +2007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>42</v>
       </c>
@@ -1993,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>42</v>
       </c>
@@ -2013,7 +2047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>42</v>
       </c>
@@ -2033,7 +2067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>42</v>
       </c>
@@ -2053,7 +2087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>42</v>
       </c>
@@ -2073,7 +2107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>42</v>
       </c>
@@ -2093,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>42</v>
       </c>
@@ -2113,7 +2147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
@@ -2133,7 +2167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
@@ -2153,7 +2187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
@@ -2173,7 +2207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>70</v>
       </c>
@@ -2193,7 +2227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>70</v>
       </c>
@@ -2213,7 +2247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>70</v>
       </c>
@@ -2233,7 +2267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -2253,7 +2287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -2273,7 +2307,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>53</v>
       </c>
@@ -2285,7 +2319,7 @@
       </c>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -2297,7 +2331,7 @@
       </c>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -2309,7 +2343,7 @@
       </c>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>53</v>
       </c>
@@ -2322,7 +2356,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>53</v>
       </c>
@@ -2334,7 +2368,7 @@
       </c>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -2346,7 +2380,7 @@
       </c>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>53</v>
       </c>
@@ -2358,7 +2392,7 @@
       </c>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>53</v>
       </c>
@@ -2370,7 +2404,7 @@
       </c>
       <c r="E81" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>71</v>
       </c>
@@ -2382,7 +2416,7 @@
       </c>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>71</v>
       </c>
@@ -2394,7 +2428,7 @@
       </c>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>71</v>
       </c>
@@ -2406,7 +2440,7 @@
       </c>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>71</v>
       </c>
@@ -2419,7 +2453,7 @@
       <c r="E86" s="6"/>
       <c r="F86" s="5"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>71</v>
       </c>
@@ -2431,7 +2465,7 @@
       </c>
       <c r="E87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>71</v>
       </c>
@@ -2443,7 +2477,7 @@
       </c>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>71</v>
       </c>
@@ -2455,7 +2489,7 @@
       </c>
       <c r="E89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>71</v>
       </c>
@@ -2480,19 +2514,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -2508,7 +2542,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>109</v>
       </c>
@@ -2521,7 +2555,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>110</v>
       </c>
@@ -2534,7 +2568,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
@@ -2544,7 +2578,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
@@ -2554,7 +2588,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
@@ -2564,7 +2598,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>19</v>
       </c>
@@ -2574,7 +2608,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
@@ -2584,7 +2618,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>19</v>
       </c>
@@ -2594,10 +2628,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -2614,7 +2648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2631,7 +2665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -2648,7 +2682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>105</v>
       </c>
@@ -2665,7 +2699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -2682,7 +2716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>106</v>
       </c>
@@ -2699,7 +2733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>107</v>
       </c>
@@ -2716,7 +2750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
@@ -2733,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
@@ -2750,12 +2784,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="D20" s="19"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -2766,7 +2800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2777,52 +2811,52 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23" s="21"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" s="21"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" s="21"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" s="21"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" s="21"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="21"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="21"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="21"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="21"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="21"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="21"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="21"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="21"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="21"/>
     </row>
   </sheetData>
@@ -2837,14 +2871,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>46</v>
       </c>
@@ -2861,7 +2895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
@@ -2870,7 +2904,7 @@
       <c r="D2" s="20"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2887,7 +2921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2904,7 +2938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2921,7 +2955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2938,7 +2972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2955,7 +2989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
@@ -2972,7 +3006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
@@ -2989,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -3006,12 +3040,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
@@ -3028,7 +3062,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -3045,7 +3079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
@@ -3062,7 +3096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>60</v>
       </c>
@@ -3079,7 +3113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
@@ -3096,7 +3130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -3113,7 +3147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -3130,7 +3164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>